<commit_message>
201106 Yichun EDA new updates
</commit_message>
<xml_diff>
--- a/02_Data/03_Policy/COVID_StatePolicy_final.xlsx
+++ b/02_Data/03_Policy/COVID_StatePolicy_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox (MIT)\2020Fall\CS109A Data Science\group assignment\CS109A_Group58\02_Data\03_Policy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F2E3F4-C886-4878-89F7-34CD89DD20B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15F9F51-54E9-40FD-A8A3-9DBD7954CECE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27525" windowHeight="10980" xr2:uid="{0B035ECF-AE5B-4B63-8BB8-57735B027CA3}"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="27525" windowHeight="10980" xr2:uid="{0B035ECF-AE5B-4B63-8BB8-57735B027CA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -486,7 +486,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -521,12 +521,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="30" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -851,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88BDAB3D-C1F9-4175-9B5E-44724F3676F4}">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="F19" workbookViewId="0">
+      <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -916,19 +910,19 @@
       <c r="M1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="R1" s="13" t="s">
         <v>119</v>
       </c>
       <c r="S1" s="1" t="s">
@@ -975,19 +969,19 @@
       <c r="M2" s="6">
         <v>43909</v>
       </c>
-      <c r="N2" s="12">
+      <c r="N2" s="6">
         <v>43951</v>
       </c>
-      <c r="O2" s="12">
+      <c r="O2" s="6">
         <v>43962</v>
       </c>
-      <c r="P2" s="12">
+      <c r="P2" s="6">
         <v>43962</v>
       </c>
-      <c r="Q2" s="12">
+      <c r="Q2" s="6">
         <v>43973</v>
       </c>
-      <c r="R2" s="12">
+      <c r="R2" s="6">
         <v>43962</v>
       </c>
       <c r="S2" s="9">
@@ -1034,19 +1028,19 @@
       <c r="M3" s="6">
         <v>43908</v>
       </c>
-      <c r="N3" s="12">
+      <c r="N3" s="6">
         <v>43945</v>
       </c>
-      <c r="O3" s="12">
+      <c r="O3" s="6">
         <v>43945</v>
       </c>
-      <c r="P3" s="12">
+      <c r="P3" s="6">
         <v>43959</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="Q3" s="6">
         <v>43959</v>
       </c>
-      <c r="R3" s="12">
+      <c r="R3" s="6">
         <v>43959</v>
       </c>
       <c r="S3" s="9">
@@ -1093,24 +1087,22 @@
       <c r="M4" s="6">
         <v>43911</v>
       </c>
-      <c r="N4" s="12">
+      <c r="N4" s="6">
         <v>43959</v>
       </c>
-      <c r="O4" s="12">
+      <c r="O4" s="6">
         <v>43962</v>
       </c>
-      <c r="P4" s="12">
+      <c r="P4" s="6">
         <v>43964</v>
       </c>
-      <c r="Q4" s="12">
+      <c r="Q4" s="6">
         <v>43967</v>
       </c>
-      <c r="R4" s="12">
+      <c r="R4" s="6">
         <v>43967</v>
       </c>
-      <c r="S4" s="8">
-        <v>0</v>
-      </c>
+      <c r="S4" s="8"/>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="1" t="s">
@@ -1125,15 +1117,11 @@
       <c r="D5" s="6">
         <v>43901</v>
       </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
+      <c r="E5" s="3"/>
       <c r="F5" s="1">
         <v>0</v>
       </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
+      <c r="G5" s="5"/>
       <c r="H5" s="6">
         <v>43907</v>
       </c>
@@ -1152,19 +1140,19 @@
       <c r="M5" s="6">
         <v>43910</v>
       </c>
-      <c r="N5" s="12">
+      <c r="N5" s="6">
         <v>43955</v>
       </c>
-      <c r="O5" s="12">
+      <c r="O5" s="6">
         <v>43962</v>
       </c>
-      <c r="P5" s="12">
+      <c r="P5" s="6">
         <v>43955</v>
       </c>
-      <c r="Q5" s="12">
+      <c r="Q5" s="6">
         <v>43969</v>
       </c>
-      <c r="R5" s="12">
+      <c r="R5" s="6">
         <v>43970</v>
       </c>
       <c r="S5" s="9">
@@ -1190,9 +1178,7 @@
       <c r="F6" s="1">
         <v>0</v>
       </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
+      <c r="G6" s="5"/>
       <c r="H6" s="6">
         <v>43913</v>
       </c>
@@ -1211,21 +1197,15 @@
       <c r="M6" s="6">
         <v>43906</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6" s="6">
         <v>43959</v>
       </c>
       <c r="O6" s="6">
         <v>43969</v>
       </c>
-      <c r="P6" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="7">
-        <v>0</v>
-      </c>
-      <c r="R6" s="7">
-        <v>0</v>
-      </c>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
       <c r="S6" s="9">
         <v>44000</v>
       </c>
@@ -1270,19 +1250,19 @@
       <c r="M7" s="6">
         <v>43907</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="6">
         <v>43952</v>
       </c>
-      <c r="O7" s="12">
+      <c r="O7" s="6">
         <v>43978</v>
       </c>
-      <c r="P7" s="12">
+      <c r="P7" s="6">
         <v>43986</v>
       </c>
-      <c r="Q7" s="12">
+      <c r="Q7" s="6">
         <v>44000</v>
       </c>
-      <c r="R7" s="12">
+      <c r="R7" s="6">
         <v>44000</v>
       </c>
       <c r="S7" s="9">
@@ -1302,9 +1282,7 @@
       <c r="D8" s="6">
         <v>43900</v>
       </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
+      <c r="E8" s="3"/>
       <c r="F8" s="1">
         <v>0</v>
       </c>
@@ -1329,21 +1307,19 @@
       <c r="M8" s="6">
         <v>43906</v>
       </c>
-      <c r="N8" s="12">
+      <c r="N8" s="6">
         <v>43971</v>
       </c>
-      <c r="O8" s="12">
+      <c r="O8" s="6">
         <v>43971</v>
       </c>
-      <c r="P8" s="12">
+      <c r="P8" s="6">
         <v>43999</v>
       </c>
-      <c r="Q8" s="12">
+      <c r="Q8" s="6">
         <v>43999</v>
       </c>
-      <c r="R8" s="7">
-        <v>0</v>
-      </c>
+      <c r="R8" s="6"/>
       <c r="S8" s="9">
         <v>43941</v>
       </c>
@@ -1388,19 +1364,19 @@
       <c r="M9" s="6">
         <v>43906</v>
       </c>
-      <c r="N9" s="12">
+      <c r="N9" s="6">
         <v>43959</v>
       </c>
-      <c r="O9" s="12">
+      <c r="O9" s="6">
         <v>43983</v>
       </c>
-      <c r="P9" s="12">
+      <c r="P9" s="6">
         <v>43983</v>
       </c>
-      <c r="Q9" s="12">
+      <c r="Q9" s="6">
         <v>43983</v>
       </c>
-      <c r="R9" s="12">
+      <c r="R9" s="6">
         <v>43997</v>
       </c>
       <c r="S9" s="9">
@@ -1447,19 +1423,19 @@
       <c r="M10" s="6">
         <v>43906</v>
       </c>
-      <c r="N10" s="12">
+      <c r="N10" s="6">
         <v>43980</v>
       </c>
-      <c r="O10" s="12">
+      <c r="O10" s="6">
         <v>43980</v>
       </c>
-      <c r="P10" s="12">
+      <c r="P10" s="6">
         <v>44004</v>
       </c>
-      <c r="Q10" s="12">
+      <c r="Q10" s="6">
         <v>44004</v>
       </c>
-      <c r="R10" s="12">
+      <c r="R10" s="6">
         <v>43980</v>
       </c>
       <c r="S10" s="9">
@@ -1506,13 +1482,13 @@
       <c r="M11" s="6">
         <v>43907</v>
       </c>
-      <c r="N11" s="12">
+      <c r="N11" s="6">
         <v>43969</v>
       </c>
-      <c r="O11" s="12">
+      <c r="O11" s="6">
         <v>43969</v>
       </c>
-      <c r="P11" s="12">
+      <c r="P11" s="6">
         <v>43969</v>
       </c>
       <c r="Q11" s="6">
@@ -1521,9 +1497,7 @@
       <c r="R11" s="6">
         <v>43987</v>
       </c>
-      <c r="S11" s="8">
-        <v>0</v>
-      </c>
+      <c r="S11" s="8"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="1" t="s">
@@ -1565,24 +1539,22 @@
       <c r="M12" s="6">
         <v>43914</v>
       </c>
-      <c r="N12" s="12">
+      <c r="N12" s="6">
         <v>43952</v>
       </c>
-      <c r="O12" s="12">
+      <c r="O12" s="6">
         <v>43948</v>
       </c>
-      <c r="P12" s="12">
+      <c r="P12" s="6">
         <v>43945</v>
       </c>
-      <c r="Q12" s="12">
+      <c r="Q12" s="6">
         <v>43948</v>
       </c>
-      <c r="R12" s="12">
+      <c r="R12" s="6">
         <v>43983</v>
       </c>
-      <c r="S12" s="8">
-        <v>0</v>
-      </c>
+      <c r="S12" s="8"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="1" t="s">
@@ -1624,24 +1596,22 @@
       <c r="M13" s="6">
         <v>43907</v>
       </c>
-      <c r="N13" s="12">
+      <c r="N13" s="6">
         <v>43958</v>
       </c>
-      <c r="O13" s="12">
+      <c r="O13" s="6">
         <v>43987</v>
       </c>
-      <c r="P13" s="12">
+      <c r="P13" s="6">
         <v>44001</v>
       </c>
-      <c r="Q13" s="12">
+      <c r="Q13" s="6">
         <v>44001</v>
       </c>
-      <c r="R13" s="12">
+      <c r="R13" s="6">
         <v>44008</v>
       </c>
-      <c r="S13" s="9">
-        <v>0</v>
-      </c>
+      <c r="S13" s="9"/>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="1" t="s">
@@ -1683,24 +1653,22 @@
       <c r="M14" s="6">
         <v>43915</v>
       </c>
-      <c r="N14" s="12">
+      <c r="N14" s="6">
         <v>43952</v>
       </c>
-      <c r="O14" s="12">
+      <c r="O14" s="6">
         <v>43967</v>
       </c>
-      <c r="P14" s="12">
+      <c r="P14" s="6">
         <v>43967</v>
       </c>
-      <c r="Q14" s="12">
+      <c r="Q14" s="6">
         <v>43981</v>
       </c>
-      <c r="R14" s="12">
+      <c r="R14" s="6">
         <v>43981</v>
       </c>
-      <c r="S14" s="8">
-        <v>0</v>
-      </c>
+      <c r="S14" s="8"/>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="1" t="s">
@@ -1742,19 +1710,19 @@
       <c r="M15" s="6">
         <v>43906</v>
       </c>
-      <c r="N15" s="12">
+      <c r="N15" s="6">
         <v>43980</v>
       </c>
-      <c r="O15" s="12">
+      <c r="O15" s="6">
         <v>43980</v>
       </c>
-      <c r="P15" s="12">
+      <c r="P15" s="6">
         <v>43980</v>
       </c>
-      <c r="Q15" s="12">
+      <c r="Q15" s="6">
         <v>44008</v>
       </c>
-      <c r="R15" s="12">
+      <c r="R15" s="6">
         <v>44008</v>
       </c>
       <c r="S15" s="9">
@@ -1801,19 +1769,19 @@
       <c r="M16" s="6">
         <v>43906</v>
       </c>
-      <c r="N16" s="12">
+      <c r="N16" s="6">
         <v>43969</v>
       </c>
-      <c r="O16" s="12">
+      <c r="O16" s="6">
         <v>43969</v>
       </c>
-      <c r="P16" s="12">
+      <c r="P16" s="6">
         <v>43983</v>
       </c>
-      <c r="Q16" s="12">
+      <c r="Q16" s="6">
         <v>43994</v>
       </c>
-      <c r="R16" s="12">
+      <c r="R16" s="6">
         <v>43994</v>
       </c>
       <c r="S16" s="9">
@@ -1833,15 +1801,11 @@
       <c r="D17" s="6">
         <v>43899</v>
       </c>
-      <c r="E17" s="3">
-        <v>0</v>
-      </c>
+      <c r="E17" s="3"/>
       <c r="F17" s="1">
         <v>0</v>
       </c>
-      <c r="G17" s="5">
-        <v>0</v>
-      </c>
+      <c r="G17" s="5"/>
       <c r="H17" s="6">
         <v>43923</v>
       </c>
@@ -1860,24 +1824,22 @@
       <c r="M17" s="6">
         <v>43907</v>
       </c>
-      <c r="N17" s="12">
+      <c r="N17" s="6">
         <v>43966</v>
       </c>
-      <c r="O17" s="12">
+      <c r="O17" s="6">
         <v>43966</v>
       </c>
-      <c r="P17" s="12">
+      <c r="P17" s="6">
         <v>43966</v>
       </c>
-      <c r="Q17" s="12">
+      <c r="Q17" s="6">
         <v>43973</v>
       </c>
-      <c r="R17" s="12">
+      <c r="R17" s="6">
         <v>43979</v>
       </c>
-      <c r="S17" s="8">
-        <v>0</v>
-      </c>
+      <c r="S17" s="8"/>
     </row>
     <row r="18" spans="1:19">
       <c r="A18" s="1" t="s">
@@ -1919,19 +1881,19 @@
       <c r="M18" s="6">
         <v>43920</v>
       </c>
-      <c r="N18" s="12">
+      <c r="N18" s="6">
         <v>43955</v>
       </c>
-      <c r="O18" s="12">
+      <c r="O18" s="6">
         <v>43955</v>
       </c>
-      <c r="P18" s="12">
+      <c r="P18" s="6">
         <v>43969</v>
       </c>
-      <c r="Q18" s="12">
+      <c r="Q18" s="6">
         <v>43973</v>
       </c>
-      <c r="R18" s="12">
+      <c r="R18" s="6">
         <v>43990</v>
       </c>
       <c r="S18" s="9">
@@ -1951,15 +1913,11 @@
       <c r="D19" s="6">
         <v>43896</v>
       </c>
-      <c r="E19" s="3">
-        <v>0</v>
-      </c>
+      <c r="E19" s="3"/>
       <c r="F19" s="1">
         <v>0</v>
       </c>
-      <c r="G19" s="5">
-        <v>0</v>
-      </c>
+      <c r="G19" s="5"/>
       <c r="H19" s="6">
         <v>43907</v>
       </c>
@@ -1978,19 +1936,19 @@
       <c r="M19" s="6">
         <v>43906</v>
       </c>
-      <c r="N19" s="12">
+      <c r="N19" s="6">
         <v>43962</v>
       </c>
-      <c r="O19" s="12">
+      <c r="O19" s="6">
         <v>43973</v>
       </c>
-      <c r="P19" s="12">
+      <c r="P19" s="6">
         <v>43983</v>
       </c>
-      <c r="Q19" s="12">
+      <c r="Q19" s="6">
         <v>43983</v>
       </c>
-      <c r="R19" s="12">
+      <c r="R19" s="6">
         <v>44011</v>
       </c>
       <c r="S19" s="9">
@@ -2037,24 +1995,22 @@
       <c r="M20" s="6">
         <v>43907</v>
       </c>
-      <c r="N20" s="12">
+      <c r="N20" s="6">
         <v>43952</v>
       </c>
-      <c r="O20" s="12">
+      <c r="O20" s="6">
         <v>43952</v>
       </c>
-      <c r="P20" s="12">
+      <c r="P20" s="6">
         <v>43966</v>
       </c>
-      <c r="Q20" s="12">
+      <c r="Q20" s="6">
         <v>43966</v>
       </c>
-      <c r="R20" s="12">
+      <c r="R20" s="6">
         <v>43987</v>
       </c>
-      <c r="S20" s="8">
-        <v>0</v>
-      </c>
+      <c r="S20" s="8"/>
     </row>
     <row r="21" spans="1:19">
       <c r="A21" s="1" t="s">
@@ -2096,19 +2052,19 @@
       <c r="M21" s="6">
         <v>43908</v>
       </c>
-      <c r="N21" s="12">
+      <c r="N21" s="6">
         <v>43952</v>
       </c>
-      <c r="O21" s="12">
+      <c r="O21" s="6">
         <v>43983</v>
       </c>
-      <c r="P21" s="12">
+      <c r="P21" s="6">
         <v>43999</v>
       </c>
-      <c r="Q21" s="12">
+      <c r="Q21" s="6">
         <v>44013</v>
       </c>
-      <c r="R21" s="12">
+      <c r="R21" s="6">
         <v>43999</v>
       </c>
       <c r="S21" s="9">
@@ -2155,19 +2111,19 @@
       <c r="M22" s="6">
         <v>43906</v>
       </c>
-      <c r="N22" s="12">
+      <c r="N22" s="6">
         <v>43966</v>
       </c>
-      <c r="O22" s="12">
+      <c r="O22" s="6">
         <v>43980</v>
       </c>
-      <c r="P22" s="12">
+      <c r="P22" s="6">
         <v>44001</v>
       </c>
-      <c r="Q22" s="12">
+      <c r="Q22" s="6">
         <v>44075</v>
       </c>
-      <c r="R22" s="12">
+      <c r="R22" s="6">
         <v>43994</v>
       </c>
       <c r="S22" s="9">
@@ -2214,21 +2170,19 @@
       <c r="M23" s="6">
         <v>43907</v>
       </c>
-      <c r="N23" s="12">
+      <c r="N23" s="6">
         <v>43969</v>
       </c>
-      <c r="O23" s="12">
+      <c r="O23" s="6">
         <v>43990</v>
       </c>
-      <c r="P23" s="12">
+      <c r="P23" s="6">
         <v>44025</v>
       </c>
-      <c r="Q23" s="12">
+      <c r="Q23" s="6">
         <v>44025</v>
       </c>
-      <c r="R23" s="7">
-        <v>0</v>
-      </c>
+      <c r="R23" s="6"/>
       <c r="S23" s="9">
         <v>43957</v>
       </c>
@@ -2273,19 +2227,19 @@
       <c r="M24" s="6">
         <v>43906</v>
       </c>
-      <c r="N24" s="12">
+      <c r="N24" s="6">
         <v>43977</v>
       </c>
-      <c r="O24" s="12">
+      <c r="O24" s="6">
         <v>43990</v>
       </c>
-      <c r="P24" s="12">
+      <c r="P24" s="6">
         <v>44083</v>
       </c>
-      <c r="Q24" s="12">
+      <c r="Q24" s="6">
         <v>44113</v>
       </c>
-      <c r="R24" s="12">
+      <c r="R24" s="6">
         <v>43990</v>
       </c>
       <c r="S24" s="9">
@@ -2332,19 +2286,19 @@
       <c r="M25" s="6">
         <v>43907</v>
       </c>
-      <c r="N25" s="12">
+      <c r="N25" s="6">
         <v>43948</v>
       </c>
-      <c r="O25" s="12">
+      <c r="O25" s="6">
         <v>43983</v>
       </c>
-      <c r="P25" s="12">
+      <c r="P25" s="6">
         <v>43992</v>
       </c>
-      <c r="Q25" s="12">
+      <c r="Q25" s="6">
         <v>43992</v>
       </c>
-      <c r="R25" s="12">
+      <c r="R25" s="6">
         <v>43992</v>
       </c>
       <c r="S25" s="9">
@@ -2391,19 +2345,19 @@
       <c r="M26" s="6">
         <v>43924</v>
       </c>
-      <c r="N26" s="12">
+      <c r="N26" s="6">
         <v>43948</v>
       </c>
-      <c r="O26" s="12">
+      <c r="O26" s="6">
         <v>43958</v>
       </c>
-      <c r="P26" s="12">
+      <c r="P26" s="6">
         <v>43962</v>
       </c>
-      <c r="Q26" s="12">
+      <c r="Q26" s="6">
         <v>43983</v>
       </c>
-      <c r="R26" s="12">
+      <c r="R26" s="6">
         <v>43983</v>
       </c>
       <c r="S26" s="9">
@@ -2450,24 +2404,20 @@
       <c r="M27" s="6">
         <v>43913</v>
       </c>
-      <c r="N27" s="12">
+      <c r="N27" s="6">
         <v>43955</v>
       </c>
-      <c r="O27" s="12">
+      <c r="O27" s="6">
         <v>43955</v>
       </c>
-      <c r="P27" s="12">
+      <c r="P27" s="6">
         <v>43955</v>
       </c>
-      <c r="Q27" s="13">
-        <v>0</v>
-      </c>
-      <c r="R27" s="12">
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6">
         <v>43955</v>
       </c>
-      <c r="S27" s="8">
-        <v>0</v>
-      </c>
+      <c r="S27" s="8"/>
     </row>
     <row r="28" spans="1:19">
       <c r="A28" s="1" t="s">
@@ -2509,24 +2459,22 @@
       <c r="M28" s="6">
         <v>43910</v>
       </c>
-      <c r="N28" s="12">
+      <c r="N28" s="6">
         <v>43948</v>
       </c>
-      <c r="O28" s="12">
+      <c r="O28" s="6">
         <v>43955</v>
       </c>
-      <c r="P28" s="12">
+      <c r="P28" s="6">
         <v>43966</v>
       </c>
-      <c r="Q28" s="12">
+      <c r="Q28" s="6">
         <v>43966</v>
       </c>
-      <c r="R28" s="12">
+      <c r="R28" s="6">
         <v>43955</v>
       </c>
-      <c r="S28" s="8">
-        <v>0</v>
-      </c>
+      <c r="S28" s="8"/>
     </row>
     <row r="29" spans="1:19">
       <c r="A29" s="1" t="s">
@@ -2541,15 +2489,11 @@
       <c r="D29" s="6">
         <v>43903</v>
       </c>
-      <c r="E29" s="3">
-        <v>0</v>
-      </c>
+      <c r="E29" s="3"/>
       <c r="F29" s="1">
         <v>0</v>
       </c>
-      <c r="G29" s="5">
-        <v>0</v>
-      </c>
+      <c r="G29" s="5"/>
       <c r="H29" s="6">
         <v>43924</v>
       </c>
@@ -2568,24 +2512,20 @@
       <c r="M29" s="6">
         <v>43924</v>
       </c>
-      <c r="N29" s="12">
+      <c r="N29" s="6">
         <v>43983</v>
       </c>
-      <c r="O29" s="12">
+      <c r="O29" s="6">
         <v>43983</v>
       </c>
-      <c r="P29" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="12">
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6">
         <v>44004</v>
       </c>
-      <c r="R29" s="12">
+      <c r="R29" s="6">
         <v>44004</v>
       </c>
-      <c r="S29" s="8">
-        <v>0</v>
-      </c>
+      <c r="S29" s="8"/>
     </row>
     <row r="30" spans="1:19">
       <c r="A30" s="1" t="s">
@@ -2627,19 +2567,19 @@
       <c r="M30" s="6">
         <v>43911</v>
       </c>
-      <c r="N30" s="12">
+      <c r="N30" s="6">
         <v>43960</v>
       </c>
-      <c r="O30" s="12">
+      <c r="O30" s="6">
         <v>43960</v>
       </c>
-      <c r="P30" s="12">
+      <c r="P30" s="6">
         <v>43980</v>
       </c>
-      <c r="Q30" s="12">
+      <c r="Q30" s="6">
         <v>43980</v>
       </c>
-      <c r="R30" s="12">
+      <c r="R30" s="6">
         <v>43980</v>
       </c>
       <c r="S30" s="9">
@@ -2686,24 +2626,22 @@
       <c r="M31" s="6">
         <v>43906</v>
       </c>
-      <c r="N31" s="12">
+      <c r="N31" s="6">
         <v>43962</v>
       </c>
-      <c r="O31" s="12">
+      <c r="O31" s="6">
         <v>43969</v>
       </c>
-      <c r="P31" s="12">
+      <c r="P31" s="6">
         <v>43983</v>
       </c>
-      <c r="Q31" s="12">
+      <c r="Q31" s="6">
         <v>44011</v>
       </c>
-      <c r="R31" s="12">
+      <c r="R31" s="6">
         <v>43997</v>
       </c>
-      <c r="S31" s="8">
-        <v>0</v>
-      </c>
+      <c r="S31" s="8"/>
     </row>
     <row r="32" spans="1:19">
       <c r="A32" s="1" t="s">
@@ -2745,19 +2683,19 @@
       <c r="M32" s="6">
         <v>43906</v>
       </c>
-      <c r="N32" s="12">
+      <c r="N32" s="6">
         <v>43969</v>
       </c>
-      <c r="O32" s="12">
+      <c r="O32" s="6">
         <v>43997</v>
       </c>
-      <c r="P32" s="12">
+      <c r="P32" s="6">
         <v>44075</v>
       </c>
-      <c r="Q32" s="12">
+      <c r="Q32" s="6">
         <v>44078</v>
       </c>
-      <c r="R32" s="12">
+      <c r="R32" s="6">
         <v>43997</v>
       </c>
       <c r="S32" s="9">
@@ -2783,9 +2721,7 @@
       <c r="F33" s="1">
         <v>1</v>
       </c>
-      <c r="G33" s="5">
-        <v>0</v>
-      </c>
+      <c r="G33" s="5"/>
       <c r="H33" s="6">
         <v>43906</v>
       </c>
@@ -2804,21 +2740,17 @@
       <c r="M33" s="6">
         <v>43909</v>
       </c>
-      <c r="N33" s="12">
+      <c r="N33" s="6">
         <v>43967</v>
       </c>
-      <c r="O33" s="12">
+      <c r="O33" s="6">
         <v>43978</v>
       </c>
-      <c r="P33" s="12">
+      <c r="P33" s="6">
         <v>43983</v>
       </c>
-      <c r="Q33" s="7">
-        <v>0</v>
-      </c>
-      <c r="R33" s="7">
-        <v>0</v>
-      </c>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
       <c r="S33" s="9">
         <v>43966</v>
       </c>
@@ -2863,21 +2795,15 @@
       <c r="M34" s="6">
         <v>43906</v>
       </c>
-      <c r="N34" s="12">
+      <c r="N34" s="6">
         <v>43990</v>
       </c>
-      <c r="O34" s="12">
+      <c r="O34" s="6">
         <v>44004</v>
       </c>
-      <c r="P34" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="7">
-        <v>0</v>
-      </c>
-      <c r="R34" s="7">
-        <v>0</v>
-      </c>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
       <c r="S34" s="9">
         <v>43938</v>
       </c>
@@ -2922,21 +2848,17 @@
       <c r="M35" s="6">
         <v>43907</v>
       </c>
-      <c r="N35" s="12">
+      <c r="N35" s="6">
         <v>43959</v>
       </c>
-      <c r="O35" s="12">
+      <c r="O35" s="6">
         <v>43973</v>
       </c>
-      <c r="P35" s="12">
+      <c r="P35" s="6">
         <v>44078</v>
       </c>
-      <c r="Q35" s="7">
-        <v>0</v>
-      </c>
-      <c r="R35" s="7">
-        <v>0</v>
-      </c>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
       <c r="S35" s="9">
         <v>44008</v>
       </c>
@@ -2954,15 +2876,11 @@
       <c r="D36" s="6">
         <v>43903</v>
       </c>
-      <c r="E36" s="3">
-        <v>0</v>
-      </c>
+      <c r="E36" s="3"/>
       <c r="F36" s="1">
         <v>0</v>
       </c>
-      <c r="G36" s="5">
-        <v>0</v>
-      </c>
+      <c r="G36" s="5"/>
       <c r="H36" s="6">
         <v>43906</v>
       </c>
@@ -2981,24 +2899,22 @@
       <c r="M36" s="6">
         <v>43910</v>
       </c>
-      <c r="N36" s="12">
+      <c r="N36" s="6">
         <v>43952</v>
       </c>
-      <c r="O36" s="12">
+      <c r="O36" s="6">
         <v>43952</v>
       </c>
-      <c r="P36" s="12">
+      <c r="P36" s="6">
         <v>43952</v>
       </c>
-      <c r="Q36" s="12">
+      <c r="Q36" s="6">
         <v>43952</v>
       </c>
-      <c r="R36" s="12">
+      <c r="R36" s="6">
         <v>43952</v>
       </c>
-      <c r="S36" s="8">
-        <v>0</v>
-      </c>
+      <c r="S36" s="8"/>
     </row>
     <row r="37" spans="1:19">
       <c r="A37" s="1" t="s">
@@ -3040,19 +2956,19 @@
       <c r="M37" s="6">
         <v>43905</v>
       </c>
-      <c r="N37" s="12">
+      <c r="N37" s="6">
         <v>43955</v>
       </c>
-      <c r="O37" s="12">
+      <c r="O37" s="6">
         <v>43966</v>
       </c>
-      <c r="P37" s="12">
+      <c r="P37" s="6">
         <v>43973</v>
       </c>
-      <c r="Q37" s="12">
+      <c r="Q37" s="6">
         <v>43992</v>
       </c>
-      <c r="R37" s="12">
+      <c r="R37" s="6">
         <v>43966</v>
       </c>
       <c r="S37" s="9">
@@ -3072,9 +2988,7 @@
       <c r="D38" s="6">
         <v>43905</v>
       </c>
-      <c r="E38" s="3">
-        <v>0</v>
-      </c>
+      <c r="E38" s="3"/>
       <c r="F38" s="1">
         <v>0</v>
       </c>
@@ -3099,24 +3013,22 @@
       <c r="M38" s="6">
         <v>43922</v>
       </c>
-      <c r="N38" s="12">
+      <c r="N38" s="6">
         <v>43945</v>
       </c>
-      <c r="O38" s="12">
+      <c r="O38" s="6">
         <v>43952</v>
       </c>
-      <c r="P38" s="12">
+      <c r="P38" s="6">
         <v>43952</v>
       </c>
-      <c r="Q38" s="12">
+      <c r="Q38" s="6">
         <v>43952</v>
       </c>
-      <c r="R38" s="12">
+      <c r="R38" s="6">
         <v>43966</v>
       </c>
-      <c r="S38" s="8">
-        <v>0</v>
-      </c>
+      <c r="S38" s="8"/>
     </row>
     <row r="39" spans="1:19">
       <c r="A39" s="1" t="s">
@@ -3158,19 +3070,17 @@
       <c r="M39" s="6">
         <v>43907</v>
       </c>
-      <c r="N39" s="12">
+      <c r="N39" s="6">
         <v>43966</v>
       </c>
-      <c r="O39" s="12">
+      <c r="O39" s="6">
         <v>44001</v>
       </c>
-      <c r="P39" s="12">
+      <c r="P39" s="6">
         <v>44001</v>
       </c>
-      <c r="Q39" s="7">
-        <v>0</v>
-      </c>
-      <c r="R39" s="12">
+      <c r="Q39" s="6"/>
+      <c r="R39" s="6">
         <v>44001</v>
       </c>
       <c r="S39" s="9">
@@ -3217,19 +3127,19 @@
       <c r="M40" s="6">
         <v>43908</v>
       </c>
-      <c r="N40" s="12">
+      <c r="N40" s="6">
         <v>43987</v>
       </c>
-      <c r="O40" s="12">
+      <c r="O40" s="6">
         <v>43987</v>
       </c>
-      <c r="P40" s="12">
+      <c r="P40" s="6">
         <v>44015</v>
       </c>
-      <c r="Q40" s="12">
+      <c r="Q40" s="6">
         <v>44015</v>
       </c>
-      <c r="R40" s="12">
+      <c r="R40" s="6">
         <v>43987</v>
       </c>
       <c r="S40" s="9">
@@ -3258,9 +3168,7 @@
       <c r="G41" s="2">
         <v>43960</v>
       </c>
-      <c r="H41" s="7">
-        <v>0</v>
-      </c>
+      <c r="H41" s="7"/>
       <c r="I41" s="6">
         <v>43920</v>
       </c>
@@ -3276,19 +3184,19 @@
       <c r="M41" s="6">
         <v>43907</v>
       </c>
-      <c r="N41" s="12">
+      <c r="N41" s="6">
         <v>43960</v>
       </c>
-      <c r="O41" s="12">
+      <c r="O41" s="6">
         <v>43969</v>
       </c>
-      <c r="P41" s="12">
+      <c r="P41" s="6">
         <v>43983</v>
       </c>
-      <c r="Q41" s="12">
+      <c r="Q41" s="6">
         <v>44012</v>
       </c>
-      <c r="R41" s="12">
+      <c r="R41" s="6">
         <v>43983</v>
       </c>
       <c r="S41" s="9">
@@ -3335,24 +3243,22 @@
       <c r="M42" s="6">
         <v>43908</v>
       </c>
-      <c r="N42" s="12">
+      <c r="N42" s="6">
         <v>43941</v>
       </c>
-      <c r="O42" s="12">
+      <c r="O42" s="6">
         <v>43955</v>
       </c>
-      <c r="P42" s="12">
+      <c r="P42" s="6">
         <v>43969</v>
       </c>
       <c r="Q42" s="6">
         <v>44046</v>
       </c>
-      <c r="R42" s="12">
+      <c r="R42" s="6">
         <v>43955</v>
       </c>
-      <c r="S42" s="8">
-        <v>0</v>
-      </c>
+      <c r="S42" s="8"/>
     </row>
     <row r="43" spans="1:19">
       <c r="A43" s="1" t="s">
@@ -3367,51 +3273,25 @@
       <c r="D43" s="6">
         <v>43903</v>
       </c>
-      <c r="E43" s="3">
-        <v>0</v>
-      </c>
+      <c r="E43" s="3"/>
       <c r="F43" s="1">
         <v>0</v>
       </c>
-      <c r="G43" s="5">
-        <v>0</v>
-      </c>
+      <c r="G43" s="5"/>
       <c r="H43" s="6">
         <v>43906</v>
       </c>
-      <c r="I43" s="8">
-        <v>0</v>
-      </c>
-      <c r="J43" s="11">
-        <v>0</v>
-      </c>
-      <c r="K43" s="7">
-        <v>0</v>
-      </c>
-      <c r="L43" s="7">
-        <v>0</v>
-      </c>
-      <c r="M43" s="7">
-        <v>0</v>
-      </c>
-      <c r="N43" s="7">
-        <v>0</v>
-      </c>
-      <c r="O43" s="7">
-        <v>0</v>
-      </c>
-      <c r="P43" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q43" s="7">
-        <v>0</v>
-      </c>
-      <c r="R43" s="7">
-        <v>0</v>
-      </c>
-      <c r="S43" s="8">
-        <v>0</v>
-      </c>
+      <c r="I43" s="8"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="6"/>
+      <c r="Q43" s="6"/>
+      <c r="R43" s="6"/>
+      <c r="S43" s="8"/>
     </row>
     <row r="44" spans="1:19">
       <c r="A44" s="1" t="s">
@@ -3453,24 +3333,22 @@
       <c r="M44" s="6">
         <v>43913</v>
       </c>
-      <c r="N44" s="12">
+      <c r="N44" s="6">
         <v>43948</v>
       </c>
-      <c r="O44" s="12">
+      <c r="O44" s="6">
         <v>43948</v>
       </c>
-      <c r="P44" s="12">
+      <c r="P44" s="6">
         <v>43952</v>
       </c>
-      <c r="Q44" s="12">
+      <c r="Q44" s="6">
         <v>43973</v>
       </c>
-      <c r="R44" s="12">
+      <c r="R44" s="6">
         <v>43973</v>
       </c>
-      <c r="S44" s="8">
-        <v>0</v>
-      </c>
+      <c r="S44" s="8"/>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" s="1" t="s">
@@ -3485,9 +3363,7 @@
       <c r="D45" s="6">
         <v>43903</v>
       </c>
-      <c r="E45" s="3">
-        <v>0</v>
-      </c>
+      <c r="E45" s="3"/>
       <c r="F45" s="1">
         <v>1</v>
       </c>
@@ -3512,19 +3388,19 @@
       <c r="M45" s="6">
         <v>43911</v>
       </c>
-      <c r="N45" s="12">
+      <c r="N45" s="6">
         <v>43952</v>
       </c>
-      <c r="O45" s="12">
+      <c r="O45" s="6">
         <v>43952</v>
       </c>
-      <c r="P45" s="12">
+      <c r="P45" s="6">
         <v>43969</v>
       </c>
-      <c r="Q45" s="12">
+      <c r="Q45" s="6">
         <v>43952</v>
       </c>
-      <c r="R45" s="12">
+      <c r="R45" s="6">
         <v>43980</v>
       </c>
       <c r="S45" s="9">
@@ -3544,15 +3420,11 @@
       <c r="D46" s="6">
         <v>43896</v>
       </c>
-      <c r="E46" s="3">
-        <v>0</v>
-      </c>
+      <c r="E46" s="3"/>
       <c r="F46" s="1">
         <v>0</v>
       </c>
-      <c r="G46" s="5">
-        <v>0</v>
-      </c>
+      <c r="G46" s="5"/>
       <c r="H46" s="6">
         <v>43906</v>
       </c>
@@ -3571,19 +3443,13 @@
       <c r="M46" s="6">
         <v>43909</v>
       </c>
-      <c r="N46" s="12">
+      <c r="N46" s="6">
         <v>43952</v>
       </c>
-      <c r="O46" s="7">
-        <v>0</v>
-      </c>
-      <c r="P46" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q46" s="7">
-        <v>0</v>
-      </c>
-      <c r="R46" s="12">
+      <c r="O46" s="6"/>
+      <c r="P46" s="6"/>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6">
         <v>43952</v>
       </c>
       <c r="S46" s="9">
@@ -3630,19 +3496,19 @@
       <c r="M47" s="6">
         <v>43907</v>
       </c>
-      <c r="N47" s="12">
+      <c r="N47" s="6">
         <v>43948</v>
       </c>
-      <c r="O47" s="12">
+      <c r="O47" s="6">
         <v>43973</v>
       </c>
-      <c r="P47" s="12">
+      <c r="P47" s="6">
         <v>43983</v>
       </c>
-      <c r="Q47" s="12">
+      <c r="Q47" s="6">
         <v>43983</v>
       </c>
-      <c r="R47" s="12">
+      <c r="R47" s="6">
         <v>43973</v>
       </c>
       <c r="S47" s="9">
@@ -3689,19 +3555,19 @@
       <c r="M48" s="6">
         <v>43915</v>
       </c>
-      <c r="N48" s="12">
+      <c r="N48" s="6">
         <v>43980</v>
       </c>
-      <c r="O48" s="12">
+      <c r="O48" s="6">
         <v>43980</v>
       </c>
-      <c r="P48" s="12">
+      <c r="P48" s="6">
         <v>43994</v>
       </c>
-      <c r="Q48" s="12">
+      <c r="Q48" s="6">
         <v>44013</v>
       </c>
-      <c r="R48" s="12">
+      <c r="R48" s="6">
         <v>43980</v>
       </c>
       <c r="S48" s="9">
@@ -3748,7 +3614,7 @@
       <c r="M49" s="6">
         <v>43907</v>
       </c>
-      <c r="N49" s="12">
+      <c r="N49" s="6">
         <v>43983</v>
       </c>
       <c r="O49" s="6">
@@ -3757,9 +3623,7 @@
       <c r="P49" s="6">
         <v>44070</v>
       </c>
-      <c r="Q49" s="7">
-        <v>0</v>
-      </c>
+      <c r="Q49" s="6"/>
       <c r="R49" s="6">
         <v>44015</v>
       </c>
@@ -3807,19 +3671,19 @@
       <c r="M50" s="6">
         <v>43908</v>
       </c>
-      <c r="N50" s="12">
+      <c r="N50" s="6">
         <v>43955</v>
       </c>
-      <c r="O50" s="12">
+      <c r="O50" s="6">
         <v>43955</v>
       </c>
-      <c r="P50" s="12">
+      <c r="P50" s="6">
         <v>43969</v>
       </c>
-      <c r="Q50" s="12">
+      <c r="Q50" s="6">
         <v>43987</v>
       </c>
-      <c r="R50" s="12">
+      <c r="R50" s="6">
         <v>43977</v>
       </c>
       <c r="S50" s="9">
@@ -3866,19 +3730,19 @@
       <c r="M51" s="6">
         <v>43907</v>
       </c>
-      <c r="N51" s="12">
+      <c r="N51" s="6">
         <v>43962</v>
       </c>
-      <c r="O51" s="12">
+      <c r="O51" s="6">
         <v>43964</v>
       </c>
-      <c r="P51" s="12">
+      <c r="P51" s="6">
         <v>43964</v>
       </c>
-      <c r="Q51" s="12">
+      <c r="Q51" s="6">
         <v>43964</v>
       </c>
-      <c r="R51" s="12">
+      <c r="R51" s="6">
         <v>43964</v>
       </c>
       <c r="S51" s="9">
@@ -3898,15 +3762,11 @@
       <c r="D52" s="6">
         <v>43903</v>
       </c>
-      <c r="E52" s="3">
-        <v>0</v>
-      </c>
+      <c r="E52" s="3"/>
       <c r="F52" s="1">
         <v>0</v>
       </c>
-      <c r="G52" s="5">
-        <v>0</v>
-      </c>
+      <c r="G52" s="5"/>
       <c r="H52" s="6">
         <v>43909</v>
       </c>
@@ -3925,27 +3785,26 @@
       <c r="M52" s="6">
         <v>43909</v>
       </c>
-      <c r="N52" s="12">
+      <c r="N52" s="6">
         <v>43952</v>
       </c>
-      <c r="O52" s="12">
+      <c r="O52" s="6">
         <v>43966</v>
       </c>
-      <c r="P52" s="12">
+      <c r="P52" s="6">
         <v>43952</v>
       </c>
-      <c r="Q52" s="12">
+      <c r="Q52" s="6">
         <v>43966</v>
       </c>
-      <c r="R52" s="12">
+      <c r="R52" s="6">
         <v>43966</v>
       </c>
-      <c r="S52" s="8">
-        <v>0</v>
-      </c>
+      <c r="S52" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>